<commit_message>
update and add grasshopper component
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="100" documentId="8_{F052ECF7-221A-452B-9A6F-3A83ECC409C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62FD0872-AF19-4938-9B32-40371C6B86B4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{8966FBC0-DB95-4302-8573-1AF5C9196750}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{8966FBC0-DB95-4302-8573-1AF5C9196750}"/>
   </bookViews>
   <sheets>
     <sheet name="IStructE | ICE V3.0 Beta 2019" sheetId="1" r:id="rId1"/>
@@ -1522,7 +1522,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>